<commit_message>
with date and \n
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -65,10 +65,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,7 +481,7 @@
     <col width="16" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>姓名</t>
@@ -499,37 +499,44 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>马太福音13-14</t>
+          <t>2月16日
+马太福音13-14</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>马太福音15-16</t>
+          <t>2月17日
+马太福音15-16</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>马太福音17-18</t>
+          <t>2月18日
+马太福音17-18</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>马太福音19-20</t>
+          <t>2月19日
+马太福音19-20</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>马太福音21-22</t>
+          <t>2月20日
+马太福音21-22</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>马太福音23-24</t>
+          <t>2月21日
+马太福音23-24</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>马太福音25-26</t>
+          <t>2月22日
+马太福音25-26</t>
         </is>
       </c>
     </row>
@@ -2290,7 +2297,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:C100">
+  <conditionalFormatting sqref="B2:B100">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>B2=7</formula>
     </cfRule>

</xml_diff>